<commit_message>
add notes and some words to excel file
</commit_message>
<xml_diff>
--- a/src/EngWordsMemo.xlsx
+++ b/src/EngWordsMemo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PawełJasiński\eclipse-workspace\memo\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC7B9843-2C5A-42A3-927B-E6B1D16EFA47}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60A10701-5556-46B2-BEC5-5B4E52FBBAB9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="204">
   <si>
     <t>thus</t>
   </si>
@@ -989,10 +989,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F148"/>
+  <dimension ref="A1:F147"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A95" workbookViewId="0">
-      <selection activeCell="D109" sqref="D109"/>
+    <sheetView tabSelected="1" topLeftCell="A128" workbookViewId="0">
+      <selection activeCell="A148" sqref="A148:G148"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3240,17 +3240,6 @@
         <v>0</v>
       </c>
     </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A148">
-        <v>147</v>
-      </c>
-      <c r="C148" t="s">
-        <v>145</v>
-      </c>
-      <c r="F148">
-        <v>0</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>